<commit_message>
xlsx data to json generation
</commit_message>
<xml_diff>
--- a/data-in/agara-mudhali-home-settings.xlsx
+++ b/data-in/agara-mudhali-home-settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\spring-boot-learning\data-jpa-sqlite\data-in\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\pdf-split-combine-app\data-in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6103673-877C-4A6B-83DC-3F160941D8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132B0CC2-0571-4953-9BF9-6E31A32D708B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>அ</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>letter</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C21" sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -494,172 +500,235 @@
     <col min="3" max="3" width="21.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
+      </c>
+      <c r="C21">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -669,21 +738,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C99D4B8-DA94-400E-B51B-54E44B73DD70}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="D1:D1048576 A1:A1048576"/>
+      <selection activeCell="F2" sqref="F2:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20.7890625" customWidth="1"/>
-    <col min="2" max="2" width="27.89453125" customWidth="1"/>
+    <col min="2" max="2" width="13.47265625" customWidth="1"/>
     <col min="3" max="3" width="22.20703125" customWidth="1"/>
     <col min="4" max="4" width="28.26171875" customWidth="1"/>
+    <col min="7" max="7" width="23.62890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -696,8 +766,14 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -711,8 +787,18 @@
         <f>CONCATENATE($C$2,"-",B2,".html")</f>
         <v>agaramudhali-1.html</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>141</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE(A2,"     ",F2)</f>
+        <v>அ     141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -724,239 +810,435 @@
         <f t="shared" ref="D3:D21" si="0">CONCATENATE($C$2,"-",B3,".html")</f>
         <v>agaramudhali-2.html</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>23</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G21" si="1">CONCATENATE(A3,"     ",F3)</f>
+        <v>ஆ     23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B21" si="1">B3+1</f>
+        <f t="shared" ref="B4:B21" si="2">B3+1</f>
         <v>3</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-3.html</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>102</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>இ     102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-4.html</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>ஈ     8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-5.html</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>உ     60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-6.html</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>ஊ     9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-7.html</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>41</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>எ     41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-8.html</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>ஏ     8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-9.html</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>ஐ     4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-10.html</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>37</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>ஒ     37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-11.html</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>ஓ     4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-12.html</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>131</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>க     131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-13.html</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>74</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>ச     74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-14.html</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>ஞ     1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-15.html</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>82</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>த     82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-16.html</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>84</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>ந     84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-17.html</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>124</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>ப     124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-18.html</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>71</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>ம     71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-19.html</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>ய     6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>agaramudhali-20.html</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <v>70</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>வ     70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22">
+        <f>SUM(F2:F21)</f>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>